<commit_message>
Cucumber default build profile
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="68">
   <si>
     <t>Create citizenship from excel</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>11_06_23_152931</t>
+  </si>
+  <si>
+    <t>11_06_23_154502</t>
+  </si>
+  <si>
+    <t>11_06_23_154510</t>
   </si>
 </sst>
 </file>
@@ -254,7 +260,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -1030,6 +1036,34 @@
         <v>65</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>